<commit_message>
fix creation of requirements
</commit_message>
<xml_diff>
--- a/src/main/resources/fenix/templates/PlantillaEspecificacionRequerimientos.xlsx
+++ b/src/main/resources/fenix/templates/PlantillaEspecificacionRequerimientos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/dminanos_everis_com/Documents/Proyectos/BMW/RSP/Fenix/1169168-Sprint 29/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\sources\popeye\src\main\resources\fenix\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>CODIGO</t>
   </si>
@@ -33,129 +33,6 @@
   </si>
   <si>
     <t>horas</t>
-  </si>
-  <si>
-    <t>STORDEV-1633</t>
-  </si>
-  <si>
-    <t>STORDEV-1740</t>
-  </si>
-  <si>
-    <t>STORDEV-1510</t>
-  </si>
-  <si>
-    <t>STORDEV-1760</t>
-  </si>
-  <si>
-    <t>STORDEV-1293</t>
-  </si>
-  <si>
-    <t>STORDEV-1764</t>
-  </si>
-  <si>
-    <t>STORDEV-1313</t>
-  </si>
-  <si>
-    <t>STORDEV-1769</t>
-  </si>
-  <si>
-    <t>STORDEV-1420</t>
-  </si>
-  <si>
-    <t>STORDEV-1421</t>
-  </si>
-  <si>
-    <t>STORDEV-1727</t>
-  </si>
-  <si>
-    <t>STORDEV-1729</t>
-  </si>
-  <si>
-    <t>STORDEV-1772</t>
-  </si>
-  <si>
-    <t>STORDEV-1644</t>
-  </si>
-  <si>
-    <t>STORDEV-1766</t>
-  </si>
-  <si>
-    <t>STORDEV-1746</t>
-  </si>
-  <si>
-    <t>Break down and coding</t>
-  </si>
-  <si>
-    <t>Code review</t>
-  </si>
-  <si>
-    <t>Merge feature branch in corresponding branch and deploy</t>
-  </si>
-  <si>
-    <t>Whenever we are sure the vehicle won¿t be touched anymore, the corresponding entry in the mapping shall be deleted.  Log when an entry is removed</t>
-  </si>
-  <si>
-    <t>Extend WLTPResponse with new fields:  co2ChargeSustaining" "description": "CO2-Ausstoß aller kombinierten Phasen." co2Weighted": "description": "Combined, weighted CO2 emissions." fuelConsumptionChargeSustaining": "description": "Kraftstoffverbrauch aller kombinierten Phasen." fuelConsumptionWeighted": "description": "Combined fuel consumption." "equivalentAllElectricRange": "description": "Rein elektrisch gefahrene Strecke aller kombinierten Phasen." "pureElectricRange: city": "description": "CO2 emissions during the load phase city." Anmerkung: alle anderen Ausprägungen von pureElectricRange sind in STOR bereits vorhanden electricConsumptionAcWeighted": ¿description": "Utility Faktor, Gewichteter elektrischer Verbrauch aus dem CD (und CS) Test." Each attribute in all properties ("comb", "low", "mid", "high", "exHigh", etc.)</t>
-  </si>
-  <si>
-    <t>In mapWLTPValues map the new values and take care of UcpV3ResponseMapperTest and EmissionSetterServiceTest either</t>
-  </si>
-  <si>
-    <t>Extend enum WltpDataField with new values.  Extend DcomFlexFieldNamesMapper.Constant  Extend mapToFlexFieldList  Create Script to add new values in DCOM_FLEX_FIELD_NAMES</t>
-  </si>
-  <si>
-    <t>extend IgDomMapper.mapWltp  extend IgDomServiceTest  extend PodIT     In orange already created and mapped  IMPEDIMENT: In blue possible error?</t>
-  </si>
-  <si>
-    <t>Use https://atc.bmwgroup.net/confluence/pages/viewpage.action?pageId=180914648&amp;preview=/180914648/225576759/vehicleEmissionV0100.xsd  to extend the vehicleEmission.class</t>
-  </si>
-  <si>
-    <t>Code Review</t>
-  </si>
-  <si>
-    <t>The class should be called from the OrderV2Resource (see STORDEV-1718).  The class is meant to be a controller between the OrderV2Resource and the IvsrServiceNewOrderRequest.doService() call.  The result object should be a OrderEnquiryResponse (STORDEV-1678).</t>
-  </si>
-  <si>
-    <t>Coding and task breakdown</t>
-  </si>
-  <si>
-    <t>Refactor and reuse the OBW IVS abstract ordering operation for use with the new VehicleOrderRequest object during Order Simulation.  This includes:  Rewiring request mappers to accept VehicleOrderRequest instead of VehicleOrder. Removing @Deprecated annotations and DeprecatedUseWarningLogger usages on classes related to this operation. Making sure that the behaviour is the same after all the changes.</t>
-  </si>
-  <si>
-    <t>OracleJDK1.8 patch for GF4 ML (STOR, DCOM,OUR)</t>
-  </si>
-  <si>
-    <t>Local IVSR Test</t>
-  </si>
-  <si>
-    <t>Deprecate unnecessary remaining classes</t>
-  </si>
-  <si>
-    <t>2.0</t>
-  </si>
-  <si>
-    <t>1.0</t>
-  </si>
-  <si>
-    <t>4.0</t>
-  </si>
-  <si>
-    <t>5.0</t>
-  </si>
-  <si>
-    <t>8.0</t>
-  </si>
-  <si>
-    <t>16.0</t>
-  </si>
-  <si>
-    <t>24.0</t>
-  </si>
-  <si>
-    <t>30.0</t>
-  </si>
-  <si>
-    <t>6.0</t>
   </si>
 </sst>
 </file>
@@ -533,7 +410,7 @@
   <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:G24"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,258 +436,122 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>40</v>
-      </c>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
       <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>38</v>
-      </c>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>38</v>
-      </c>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>40</v>
-      </c>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
       <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>38</v>
-      </c>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>40</v>
-      </c>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>38</v>
-      </c>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>38</v>
-      </c>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>38</v>
-      </c>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>38</v>
-      </c>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>38</v>
-      </c>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>41</v>
-      </c>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>42</v>
-      </c>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>40</v>
-      </c>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>43</v>
-      </c>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>44</v>
-      </c>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>38</v>
-      </c>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
       <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>